<commit_message>
update for lower board and driver.
</commit_message>
<xml_diff>
--- a/document/System Main Design Document.xlsx
+++ b/document/System Main Design Document.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user_project\git\remote_manage\document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375C9B30-2C1F-4CD2-9AAA-2EEA038D0F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12690" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="开发模块" sheetId="5" r:id="rId1"/>
@@ -142,7 +148,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Cambria"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -158,7 +164,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Cambria"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -217,7 +223,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Cambria"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -320,7 +326,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Cambria"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -881,39 +887,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -930,153 +930,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -1099,7 +955,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1108,198 +964,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.399975585192419"/>
+        <fgColor theme="3" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1396,251 +1078,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1652,15 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1684,17 +1115,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1708,62 +1130,36 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2050,21 +1446,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.0916666666667" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2114,251 +1510,247 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="75.45" style="20" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="21"/>
+    <col min="1" max="1" width="75.453125" style="14" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="30" spans="1:1">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:1" ht="29">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="90" spans="1:1">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:1" ht="87">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" ht="45" spans="1:1">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:1" ht="43.5">
+      <c r="A15" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" ht="45" spans="1:1">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:1" ht="43.5">
+      <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" ht="75" spans="1:1">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:1" ht="87">
+      <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" ht="123.5" customHeight="1" spans="1:1">
-      <c r="A24" s="20" t="s">
+    <row r="24" spans="1:1" ht="123.5" customHeight="1">
+      <c r="A24" s="14" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.5416666666667" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.45" style="3" customWidth="1"/>
-    <col min="3" max="3" width="69.725" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.725" style="3"/>
+    <col min="1" max="1" width="22.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="69.7265625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" ht="40.5" spans="1:3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:4" ht="42">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" ht="27" spans="1:3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:4" ht="28">
+      <c r="A3" s="18"/>
+      <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" ht="54" spans="1:3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="1:4" ht="56">
+      <c r="A4" s="18"/>
+      <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" ht="108" spans="1:3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:4" ht="112">
+      <c r="A5" s="18"/>
+      <c r="B5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" ht="31.5" spans="1:4">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:4" ht="31.5">
+      <c r="A6" s="18"/>
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" ht="40.5" spans="1:4">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="42">
+      <c r="A7" s="18"/>
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="17"/>
-    </row>
-    <row r="8" ht="27" spans="1:4">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" ht="28">
+      <c r="A8" s="18"/>
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" ht="40.5" spans="1:4">
-      <c r="A9" s="18"/>
-      <c r="B9" s="14" t="s">
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="42">
+      <c r="A9" s="19"/>
+      <c r="B9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" ht="27" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" ht="28">
+      <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="18"/>
+      <c r="B11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" ht="27" spans="1:3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="18"/>
+      <c r="B12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" ht="67.5" spans="1:3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="1:4" ht="70">
+      <c r="A13" s="19"/>
+      <c r="B13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2368,63 +1760,61 @@
     <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.9083333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.725" customWidth="1"/>
-    <col min="5" max="5" width="24.8166666666667" customWidth="1"/>
-    <col min="6" max="6" width="25.0916666666667" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.08984375" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.2666666666667" customWidth="1"/>
-    <col min="10" max="10" width="20.8166666666667" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="11.2666666666667" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="E1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I2" t="s">
@@ -2432,22 +1822,22 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>57</v>
       </c>
       <c r="I3" t="s">
@@ -2455,22 +1845,22 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>57</v>
       </c>
       <c r="I4" t="s">
@@ -2478,469 +1868,469 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="10" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="E14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="8" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="B20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="C25" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" s="9" t="s">
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="C26" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="9" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="9" t="s">
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="9" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="10" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="9" t="s">
         <v>137</v>
       </c>
       <c r="B39" t="s">
@@ -2949,11 +2339,11 @@
       <c r="C39" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9" t="s">
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2967,15 +2357,15 @@
       <c r="C40" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9" t="s">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>142</v>
       </c>
@@ -2986,7 +2376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>144</v>
       </c>
@@ -2994,7 +2384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -3005,7 +2395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -3013,8 +2403,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="13">
+    <row r="45" spans="1:7">
+      <c r="A45" s="10">
         <v>485</v>
       </c>
       <c r="B45" t="s">
@@ -3024,7 +2414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -3035,7 +2425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>151</v>
       </c>
@@ -3046,7 +2436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -3233,34 +2623,32 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 G3:G19 G39:G40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 G3:G19 G39:G40" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$I$2:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" style="3" customWidth="1"/>
-    <col min="2" max="2" width="54.8166666666667" style="3" customWidth="1"/>
-    <col min="3" max="3" width="67.3666666666667" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.725" style="3"/>
+    <col min="2" max="2" width="54.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="67.36328125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="40.5" spans="1:2">
+    <row r="1" spans="1:3" ht="43.5">
       <c r="A1" s="3" t="s">
         <v>177</v>
       </c>
@@ -3279,7 +2667,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" ht="54" spans="1:3">
+    <row r="3" spans="1:3" ht="58">
       <c r="A3" s="3" t="s">
         <v>181</v>
       </c>
@@ -3290,7 +2678,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" ht="108" spans="1:3">
+    <row r="4" spans="1:3" ht="116">
       <c r="A4" s="3" t="s">
         <v>184</v>
       </c>
@@ -3301,7 +2689,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" ht="40.5" spans="1:3">
+    <row r="5" spans="1:3" ht="43.5">
       <c r="A5" s="3" t="s">
         <v>187</v>
       </c>
@@ -3314,23 +2702,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="42.0916666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.08984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3415,7 +2801,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
support for dac, adc capture.
</commit_message>
<xml_diff>
--- a/document/System Main Design Document.xlsx
+++ b/document/System Main Design Document.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user_project\git\remote_manage\document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375C9B30-2C1F-4CD2-9AAA-2EEA038D0F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="12690" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="开发模块" sheetId="5" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="205">
   <si>
     <t>嵌入式软件</t>
   </si>
@@ -148,7 +142,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -164,7 +158,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -223,7 +217,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -326,7 +320,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -556,9 +550,6 @@
     <t>ADC</t>
   </si>
   <si>
-    <t>ADC+DMA</t>
-  </si>
-  <si>
     <t>LCD背光条件</t>
   </si>
   <si>
@@ -887,33 +878,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.15"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -930,9 +934,153 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -955,7 +1103,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -964,24 +1112,210 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39994506668294322"/>
+        <fgColor theme="3" tint="0.399945066682943"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1078,11 +1412,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1093,73 +1669,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1446,21 +2070,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="1" max="1" width="23.0916666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1510,247 +2134,251 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="75.453125" style="14" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="15"/>
+    <col min="1" max="1" width="75.45" style="22" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="29">
-      <c r="A3" s="14" t="s">
+    <row r="3" ht="30" spans="1:1">
+      <c r="A3" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="87">
-      <c r="A6" s="14" t="s">
+    <row r="6" ht="90" spans="1:1">
+      <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="43.5">
-      <c r="A15" s="14" t="s">
+    <row r="15" ht="45" spans="1:1">
+      <c r="A15" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="43.5">
-      <c r="A18" s="14" t="s">
+    <row r="18" ht="45" spans="1:1">
+      <c r="A18" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="87">
-      <c r="A21" s="14" t="s">
+    <row r="21" ht="75" spans="1:1">
+      <c r="A21" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="123.5" customHeight="1">
-      <c r="A24" s="14" t="s">
+    <row r="24" ht="123.5" customHeight="1" spans="1:1">
+      <c r="A24" s="22" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="69.7265625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="22.5416666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.45" style="3" customWidth="1"/>
+    <col min="3" max="3" width="69.725" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42">
+    <row r="2" ht="40.5" spans="1:3">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
+    <row r="3" ht="27" spans="1:3">
       <c r="A3" s="18"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56">
+    <row r="4" ht="54" spans="1:3">
       <c r="A4" s="18"/>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="112">
+    <row r="5" ht="108" spans="1:3">
       <c r="A5" s="18"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5">
+    <row r="6" ht="31.5" spans="1:4">
       <c r="A6" s="18"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="42">
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" ht="40.5" spans="1:4">
       <c r="A7" s="18"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="28">
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" ht="27" spans="1:4">
       <c r="A8" s="18"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="42">
-      <c r="A9" s="19"/>
-      <c r="B9" s="11" t="s">
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" ht="40.5" spans="1:4">
+      <c r="A9" s="20"/>
+      <c r="B9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4" ht="28">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" ht="27" spans="1:3">
       <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11" s="18"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" ht="27" spans="1:3">
       <c r="A12" s="18"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="70">
-      <c r="A13" s="19"/>
-      <c r="B13" s="11" t="s">
+    <row r="13" ht="67.5" spans="1:3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1760,61 +2388,63 @@
     <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.9083333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.725" customWidth="1"/>
+    <col min="5" max="5" width="24.8166666666667" customWidth="1"/>
+    <col min="6" max="6" width="25.0916666666667" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.2666666666667" customWidth="1"/>
+    <col min="10" max="10" width="20.8166666666667" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" customWidth="1"/>
+    <col min="12" max="12" width="11.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="7" t="s">
         <v>56</v>
       </c>
       <c r="I2" t="s">
@@ -1822,22 +2452,22 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I3" t="s">
@@ -1845,22 +2475,22 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I4" t="s">
@@ -1868,470 +2498,470 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="5" t="s">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="B23" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="7" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="B39" t="s">
         <v>55</v>
@@ -2339,109 +2969,109 @@
       <c r="C39" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6" t="s">
+      <c r="E39" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" t="s">
         <v>139</v>
-      </c>
-      <c r="B40" t="s">
-        <v>140</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>141</v>
       </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>142</v>
-      </c>
-      <c r="B41" t="s">
-        <v>143</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" t="s">
         <v>145</v>
-      </c>
-      <c r="B43" t="s">
-        <v>146</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="10">
+    <row r="45" spans="1:3">
+      <c r="A45" s="15">
         <v>485</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" t="s">
         <v>149</v>
-      </c>
-      <c r="B46" t="s">
-        <v>150</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" t="s">
         <v>152</v>
-      </c>
-      <c r="B48" t="s">
-        <v>153</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -2449,10 +3079,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" t="s">
         <v>154</v>
-      </c>
-      <c r="B49" t="s">
-        <v>155</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -2460,10 +3090,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" t="s">
         <v>156</v>
-      </c>
-      <c r="B50" t="s">
-        <v>157</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
@@ -2471,10 +3101,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
@@ -2482,10 +3112,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
@@ -2493,7 +3123,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
         <v>100</v>
@@ -2504,10 +3134,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" t="s">
         <v>161</v>
-      </c>
-      <c r="B54" t="s">
-        <v>162</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
@@ -2515,7 +3145,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -2523,7 +3153,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2531,10 +3161,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" t="s">
         <v>165</v>
-      </c>
-      <c r="B57" t="s">
-        <v>166</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2542,10 +3172,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2553,10 +3183,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
@@ -2564,10 +3194,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
@@ -2575,10 +3205,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -2586,10 +3216,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" t="s">
         <v>171</v>
-      </c>
-      <c r="B62" t="s">
-        <v>172</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -2597,21 +3227,21 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" t="s">
         <v>173</v>
-      </c>
-      <c r="B63" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" t="s">
         <v>175</v>
-      </c>
-      <c r="B64" t="s">
-        <v>176</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
@@ -2623,184 +3253,189 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 G3:G19 G39:G40" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 G3:G19 G39:G40">
       <formula1>$I$2:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="20" style="3" customWidth="1"/>
-    <col min="2" max="2" width="54.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="67.36328125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="54.8166666666667" style="3" customWidth="1"/>
+    <col min="3" max="3" width="67.3666666666667" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.5">
+    <row r="1" ht="40.5" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" ht="54" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="58">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="4" ht="108" spans="1:3">
+      <c r="A4" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="116">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" ht="40.5" spans="1:3">
+      <c r="A5" s="3" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.5">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="42.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.0916666666667" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[lower_app]update for spi support.
</commit_message>
<xml_diff>
--- a/document/System Main Design Document.xlsx
+++ b/document/System Main Design Document.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user_project\git\remote_manage\document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63720048-68A3-4F8C-A279-33C8DD5BFA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="12690" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="开发模块" sheetId="5" r:id="rId1"/>
@@ -148,7 +142,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -164,7 +158,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -223,7 +217,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -326,7 +320,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="major"/>
       </rPr>
@@ -619,154 +613,154 @@
     <t>字库</t>
   </si>
   <si>
+    <t>FPU测试</t>
+  </si>
+  <si>
+    <t>fpu</t>
+  </si>
+  <si>
+    <t>DSP测试</t>
+  </si>
+  <si>
+    <t>dsp</t>
+  </si>
+  <si>
+    <t>串口IAP实验</t>
+  </si>
+  <si>
+    <t>IAP</t>
+  </si>
+  <si>
+    <t>FreeRTOS相关</t>
+  </si>
+  <si>
+    <t>rtos</t>
+  </si>
+  <si>
+    <t>单片机硬件</t>
+  </si>
+  <si>
+    <t>WIFI驱动</t>
+  </si>
+  <si>
+    <t>窗口看门狗</t>
+  </si>
+  <si>
+    <t>WWDG</t>
+  </si>
+  <si>
+    <t>4G通讯</t>
+  </si>
+  <si>
+    <t>TFTLCD(RGB屏)</t>
+  </si>
+  <si>
+    <t>LTDC</t>
+  </si>
+  <si>
+    <t>USMART调试组件</t>
+  </si>
+  <si>
+    <t>OLED显示</t>
+  </si>
+  <si>
+    <t>并口IO模拟</t>
+  </si>
+  <si>
+    <t>待机唤醒</t>
+  </si>
+  <si>
+    <t>UART+RS485</t>
+  </si>
+  <si>
+    <t>DS18B20</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>DH11数字湿度传感器</t>
+  </si>
+  <si>
+    <t>无线通讯</t>
+  </si>
+  <si>
+    <t>SPI+NRF24L01</t>
+  </si>
+  <si>
+    <t>摄像头</t>
+  </si>
+  <si>
+    <t>DCMI</t>
+  </si>
+  <si>
+    <t>内存管理</t>
+  </si>
+  <si>
+    <t>malloc/free</t>
+  </si>
+  <si>
+    <t>照相机</t>
+  </si>
+  <si>
+    <t>音乐播放器</t>
+  </si>
+  <si>
+    <t>录音机</t>
+  </si>
+  <si>
+    <t>视频播放</t>
+  </si>
+  <si>
+    <t>Mege</t>
+  </si>
+  <si>
+    <t>手写识别</t>
+  </si>
+  <si>
+    <t>T9拼音输入法</t>
+  </si>
+  <si>
+    <t>USB读卡器(Slave)</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>USB声卡(Slave)</t>
+  </si>
+  <si>
+    <t>USB虚拟串口(slave)</t>
+  </si>
+  <si>
+    <t>USB U盘(Host)</t>
+  </si>
+  <si>
+    <t>USB 鼠标键盘(Host)</t>
+  </si>
+  <si>
+    <t>网络通讯</t>
+  </si>
+  <si>
+    <t>ETH/LWIP</t>
+  </si>
+  <si>
+    <t>PWM DAC</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>红外遥控</t>
+  </si>
+  <si>
+    <t>Timer Capture</t>
+  </si>
+  <si>
     <t>图片显示</t>
   </si>
   <si>
     <t>图像</t>
-  </si>
-  <si>
-    <t>FPU测试</t>
-  </si>
-  <si>
-    <t>fpu</t>
-  </si>
-  <si>
-    <t>DSP测试</t>
-  </si>
-  <si>
-    <t>dsp</t>
-  </si>
-  <si>
-    <t>串口IAP实验</t>
-  </si>
-  <si>
-    <t>IAP</t>
-  </si>
-  <si>
-    <t>FreeRTOS相关</t>
-  </si>
-  <si>
-    <t>rtos</t>
-  </si>
-  <si>
-    <t>单片机硬件</t>
-  </si>
-  <si>
-    <t>WIFI驱动</t>
-  </si>
-  <si>
-    <t>窗口看门狗</t>
-  </si>
-  <si>
-    <t>WWDG</t>
-  </si>
-  <si>
-    <t>4G通讯</t>
-  </si>
-  <si>
-    <t>TFTLCD(RGB屏)</t>
-  </si>
-  <si>
-    <t>LTDC</t>
-  </si>
-  <si>
-    <t>USMART调试组件</t>
-  </si>
-  <si>
-    <t>OLED显示</t>
-  </si>
-  <si>
-    <t>并口IO模拟</t>
-  </si>
-  <si>
-    <t>待机唤醒</t>
-  </si>
-  <si>
-    <t>UART+RS485</t>
-  </si>
-  <si>
-    <t>DS18B20</t>
-  </si>
-  <si>
-    <t>I/O</t>
-  </si>
-  <si>
-    <t>DH11数字湿度传感器</t>
-  </si>
-  <si>
-    <t>无线通讯</t>
-  </si>
-  <si>
-    <t>SPI+NRF24L01</t>
-  </si>
-  <si>
-    <t>摄像头</t>
-  </si>
-  <si>
-    <t>DCMI</t>
-  </si>
-  <si>
-    <t>内存管理</t>
-  </si>
-  <si>
-    <t>malloc/free</t>
-  </si>
-  <si>
-    <t>照相机</t>
-  </si>
-  <si>
-    <t>音乐播放器</t>
-  </si>
-  <si>
-    <t>录音机</t>
-  </si>
-  <si>
-    <t>视频播放</t>
-  </si>
-  <si>
-    <t>Mege</t>
-  </si>
-  <si>
-    <t>手写识别</t>
-  </si>
-  <si>
-    <t>T9拼音输入法</t>
-  </si>
-  <si>
-    <t>USB读卡器(Slave)</t>
-  </si>
-  <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>USB声卡(Slave)</t>
-  </si>
-  <si>
-    <t>USB虚拟串口(slave)</t>
-  </si>
-  <si>
-    <t>USB U盘(Host)</t>
-  </si>
-  <si>
-    <t>USB 鼠标键盘(Host)</t>
-  </si>
-  <si>
-    <t>网络通讯</t>
-  </si>
-  <si>
-    <t>ETH/LWIP</t>
-  </si>
-  <si>
-    <t>PWM DAC</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
-    <t>红外遥控</t>
-  </si>
-  <si>
-    <t>Timer Capture</t>
   </si>
   <si>
     <t>扩展</t>
@@ -872,40 +866,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Calibri"/>
+      <color theme="0" tint="-0.149998474074526"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -922,9 +922,153 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -947,7 +1091,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,24 +1100,210 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39991454817346722"/>
+        <fgColor theme="3" tint="0.399914548173467"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1070,9 +1400,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1085,6 +1657,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1111,8 +1692,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1126,36 +1716,62 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1442,21 +2058,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="1" max="1" width="23.0916666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1506,247 +2122,251 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="75.453125" style="16" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="17"/>
+    <col min="1" max="1" width="75.45" style="22" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="29">
-      <c r="A3" s="16" t="s">
+    <row r="3" ht="30" spans="1:1">
+      <c r="A3" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="87">
-      <c r="A6" s="16" t="s">
+    <row r="6" ht="90" spans="1:1">
+      <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="43.5">
-      <c r="A15" s="16" t="s">
+    <row r="15" ht="45" spans="1:1">
+      <c r="A15" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="43.5">
-      <c r="A18" s="16" t="s">
+    <row r="18" ht="45" spans="1:1">
+      <c r="A18" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="87">
-      <c r="A21" s="16" t="s">
+    <row r="21" ht="75" spans="1:1">
+      <c r="A21" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="123.5" customHeight="1">
-      <c r="A24" s="16" t="s">
+    <row r="24" ht="123.5" customHeight="1" spans="1:1">
+      <c r="A24" s="22" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="69.7265625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="22.5416666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45.45" style="3" customWidth="1"/>
+    <col min="3" max="3" width="69.725" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42">
-      <c r="A2" s="19" t="s">
+    <row r="2" ht="40.5" spans="1:3">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28">
-      <c r="A3" s="20"/>
-      <c r="B3" s="13" t="s">
+    <row r="3" ht="27" spans="1:3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56">
-      <c r="A4" s="20"/>
-      <c r="B4" s="13" t="s">
+    <row r="4" ht="54" spans="1:3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="112">
-      <c r="A5" s="20"/>
-      <c r="B5" s="13" t="s">
+    <row r="5" ht="108" spans="1:3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5">
-      <c r="A6" s="20"/>
-      <c r="B6" s="13" t="s">
+    <row r="6" ht="31.5" spans="1:4">
+      <c r="A6" s="18"/>
+      <c r="B6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4" ht="42">
-      <c r="A7" s="20"/>
-      <c r="B7" s="13" t="s">
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" ht="40.5" spans="1:4">
+      <c r="A7" s="18"/>
+      <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:4" ht="28">
-      <c r="A8" s="20"/>
-      <c r="B8" s="13" t="s">
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" ht="27" spans="1:4">
+      <c r="A8" s="18"/>
+      <c r="B8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:4" ht="42">
-      <c r="A9" s="21"/>
-      <c r="B9" s="13" t="s">
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" ht="40.5" spans="1:4">
+      <c r="A9" s="20"/>
+      <c r="B9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="28">
-      <c r="A10" s="19" t="s">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" ht="27" spans="1:3">
+      <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="20"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="20"/>
-      <c r="B12" s="13" t="s">
+    <row r="12" ht="27" spans="1:3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="70">
-      <c r="A13" s="21"/>
-      <c r="B13" s="13" t="s">
+    <row r="13" ht="67.5" spans="1:3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1756,61 +2376,63 @@
     <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.9083333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.725" customWidth="1"/>
+    <col min="5" max="5" width="24.8166666666667" customWidth="1"/>
+    <col min="6" max="6" width="25.0916666666667" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.2666666666667" customWidth="1"/>
+    <col min="10" max="10" width="20.8166666666667" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" customWidth="1"/>
+    <col min="12" max="12" width="11.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="7" t="s">
         <v>56</v>
       </c>
       <c r="I2" t="s">
@@ -1818,22 +2440,22 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I3" t="s">
@@ -1841,22 +2463,22 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I4" t="s">
@@ -1864,437 +2486,426 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B31" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="7" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="5" t="s">
+      <c r="C33" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="B36" t="s">
         <v>55</v>
@@ -2302,142 +2913,142 @@
       <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7" t="s">
+      <c r="E36" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
         <v>136</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>137</v>
-      </c>
-      <c r="B38" t="s">
-        <v>138</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="12">
+    <row r="42" spans="1:3">
+      <c r="A42" s="15">
         <v>485</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -2445,7 +3056,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
         <v>107</v>
@@ -2456,7 +3067,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
         <v>100</v>
@@ -2467,10 +3078,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
@@ -2478,7 +3089,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
@@ -2486,7 +3097,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
@@ -2494,10 +3105,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
@@ -2505,10 +3116,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -2516,10 +3127,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2527,10 +3138,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2538,10 +3149,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2549,10 +3160,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
@@ -2560,23 +3171,34 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
         <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2586,32 +3208,34 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G19 G36:G37 C3:C33" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C62 C3:C28 C30:C33 G3:G19 G36:G37">
       <formula1>$I$2:$I$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="20" style="3" customWidth="1"/>
-    <col min="2" max="2" width="54.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="67.36328125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="54.8166666666667" style="3" customWidth="1"/>
+    <col min="3" max="3" width="67.3666666666667" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.5">
+    <row r="1" ht="40.5" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>172</v>
       </c>
@@ -2630,7 +3254,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="58">
+    <row r="3" ht="54" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>176</v>
       </c>
@@ -2641,7 +3265,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="116">
+    <row r="4" ht="108" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>179</v>
       </c>
@@ -2652,7 +3276,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.5">
+    <row r="5" ht="40.5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>182</v>
       </c>
@@ -2665,21 +3289,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="42.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.0916666666667" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2764,6 +3390,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 

</xml_diff>